<commit_message>
Revert "Přidány nové funkce"
This reverts commit 81544cfe2396dffee023396df2ad321ca3b9c72e.
</commit_message>
<xml_diff>
--- a/Excel pro program.xlsx
+++ b/Excel pro program.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programování\Chytré nástroje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2014B64F-7A09-4EE1-BEF9-7CF4AAACEFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5070DD1-D8AC-45A5-A1BF-F7D06D4270C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B91DDEB3-73B7-415D-A1F4-216134C04092}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>Nikodémová Eliška</t>
   </si>
   <si>
-    <t>programnovy</t>
+    <t>NOVÁK Jakub</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,20 +601,23 @@
         <v>18</v>
       </c>
       <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3">IFERROR(_xlfn.TEXTSPLIT(A3," "," "),"Nejsou hodnoty")</f>
-        <v>programnovy</v>
+        <f t="array" ref="B3:C3">IFERROR(_xlfn.TEXTSPLIT(A3," "," "),"Nejsou hodnoty")</f>
+        <v>NOVÁK</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Jakub</v>
       </c>
       <c r="D3" t="str">
         <f>IF(C3="","Nejsou hodnoty", C3)</f>
-        <v>Nejsou hodnoty</v>
+        <v>Jakub</v>
       </c>
       <c r="E3" t="str">
         <f>IF(B3="Nejsou hodnoty", B3, PROPER(B3))</f>
-        <v>Programnovy</v>
-      </c>
-      <c r="F3" t="e" cm="1">
-        <f t="array" aca="1" ref="F3" ca="1">IF(A4="","Nejsou hodnoty",(LOWER(E3))&amp;OdstranitDiakritiku(LOWER(D3)))</f>
-        <v>#NAME?</v>
+        <v>Novák</v>
+      </c>
+      <c r="F3" t="str" cm="1">
+        <f t="array" ref="F3">IF(A4="","Nejsou hodnoty",OdstranitDiakritiku(LOWER(E3))&amp;OdstranitDiakritiku(LOWER(D3)))</f>
+        <v>novakjakub</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>